<commit_message>
Started adding Pub Invoice Tracker and other
</commit_message>
<xml_diff>
--- a/DibsOrderMgmt/HiveTemplates/HIVE_PackingSlip_Template.xlsx
+++ b/DibsOrderMgmt/HiveTemplates/HIVE_PackingSlip_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\MEP - Shared\BrainHive\BH_OrderMgmt\HIVE_Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RickyHarlow\source\repos\DibsOrderMgmt\DibsOrderMgmt\HiveTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05294608-BCC7-486A-A934-90502DFD495A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174A22DE-D4FA-4E27-BC62-28CE98D91C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12239" uniqueCount="3817">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12238" uniqueCount="3816">
   <si>
     <t>1_ISBN</t>
   </si>
@@ -11951,18 +11951,12 @@
     <t xml:space="preserve">PO NUMBER </t>
   </si>
   <si>
-    <t>DATE:</t>
-  </si>
-  <si>
     <t>aharlow@myedupartners.com</t>
   </si>
   <si>
     <t>Amber Harlow</t>
   </si>
   <si>
-    <t>919.395.7315</t>
-  </si>
-  <si>
     <t>Questions?</t>
   </si>
   <si>
@@ -11979,6 +11973,9 @@
   </si>
   <si>
     <t>Item Number</t>
+  </si>
+  <si>
+    <t>Date:</t>
   </si>
 </sst>
 </file>
@@ -11992,7 +11989,7 @@
     <numFmt numFmtId="166" formatCode="m/d"/>
     <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="38" x14ac:knownFonts="1">
+  <fonts count="36" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -12180,12 +12177,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -12233,14 +12224,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -12354,7 +12337,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
@@ -12363,12 +12346,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -12643,123 +12625,119 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="7"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1"/>
-    <xf numFmtId="15" fontId="21" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="7" applyFont="1"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="8" applyFont="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="7" applyFont="1"/>
+    <xf numFmtId="15" fontId="21" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="7" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="7" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="7" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="6" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="6" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="27" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="12" fontId="19" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="12" fontId="19" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="12" fontId="19" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="28" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="19" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="19" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="12" fontId="19" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="28" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="19" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="10">
-    <cellStyle name="Currency" xfId="6" builtinId="4"/>
-    <cellStyle name="Currency 2" xfId="8" xr:uid="{6B92F9BA-6954-464D-B1F8-2E84871F6C8B}"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8"/>
+  <cellStyles count="9">
+    <cellStyle name="Currency 2" xfId="7" xr:uid="{6B92F9BA-6954-464D-B1F8-2E84871F6C8B}"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 11" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Normal 3" xfId="7" xr:uid="{B445A6A5-1882-486D-9BE8-B538B2B09C37}"/>
+    <cellStyle name="Normal 3" xfId="6" xr:uid="{B445A6A5-1882-486D-9BE8-B538B2B09C37}"/>
     <cellStyle name="Normal 6" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Normal 8" xfId="2" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
   </cellStyles>
@@ -13337,10 +13315,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1693FC4-EBD1-4A4B-9B78-1EAAE4715BC1}">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -13348,110 +13326,101 @@
     <col min="1" max="1" width="13.5" style="120" customWidth="1"/>
     <col min="2" max="2" width="15.875" style="120" customWidth="1"/>
     <col min="3" max="3" width="46.75" style="120" customWidth="1"/>
-    <col min="4" max="4" width="10.375" style="120" customWidth="1"/>
-    <col min="5" max="5" width="6.625" style="120" customWidth="1"/>
-    <col min="6" max="6" width="9" style="120"/>
-    <col min="7" max="7" width="15" style="110" customWidth="1"/>
-    <col min="8" max="8" width="10.125" style="111" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9" style="110"/>
-    <col min="11" max="11" width="14.75" style="110" customWidth="1"/>
-    <col min="12" max="12" width="15" style="110" customWidth="1"/>
-    <col min="13" max="16384" width="9" style="110"/>
+    <col min="4" max="4" width="6.625" style="120" customWidth="1"/>
+    <col min="5" max="5" width="9" style="120"/>
+    <col min="6" max="6" width="15" style="110" customWidth="1"/>
+    <col min="7" max="7" width="10.125" style="111" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9" style="110"/>
+    <col min="10" max="10" width="14.75" style="110" customWidth="1"/>
+    <col min="11" max="11" width="15" style="110" customWidth="1"/>
+    <col min="12" max="16384" width="9" style="110"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="144" t="s">
-        <v>3812</v>
-      </c>
-      <c r="B1" s="144" t="s">
+    <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="150" t="s">
+        <v>3810</v>
+      </c>
+      <c r="B1" s="150" t="s">
         <v>3795</v>
       </c>
-      <c r="C1" s="144"/>
-      <c r="D1" s="144"/>
-      <c r="E1" s="144" t="s">
+      <c r="C1" s="150"/>
+      <c r="D1" s="150" t="s">
         <v>3795</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="124" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="124" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="122"/>
       <c r="B2" s="122"/>
       <c r="C2" s="123" t="s">
         <v>3802</v>
       </c>
-      <c r="E2" s="123"/>
-      <c r="F2" s="126"/>
-      <c r="H2" s="125"/>
-    </row>
-    <row r="3" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="123"/>
+      <c r="E2" s="126"/>
+      <c r="G2" s="125"/>
+    </row>
+    <row r="3" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="127"/>
       <c r="B3" s="112"/>
       <c r="C3" s="116" t="s">
         <v>3803</v>
       </c>
-      <c r="E3" s="116"/>
-    </row>
-    <row r="4" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="116"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="118"/>
       <c r="B4" s="113"/>
       <c r="C4" s="116" t="s">
         <v>3800</v>
       </c>
-      <c r="E4" s="116"/>
-    </row>
-    <row r="5" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="116"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="127"/>
       <c r="B5" s="113"/>
       <c r="C5" s="116" t="s">
         <v>3801</v>
       </c>
-      <c r="E5" s="116"/>
-    </row>
-    <row r="6" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="116"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="118"/>
       <c r="B6" s="113"/>
       <c r="C6" s="113"/>
-      <c r="D6" s="150"/>
-      <c r="E6" s="151"/>
-    </row>
-    <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="118"/>
-      <c r="B7" s="113"/>
+      <c r="D6" s="143"/>
+    </row>
+    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="139" t="s">
+        <v>3815</v>
+      </c>
+      <c r="B7" s="116"/>
       <c r="C7" s="113"/>
-      <c r="D7" s="146"/>
-      <c r="E7" s="146"/>
-    </row>
-    <row r="8" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="141"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="119" t="s">
-        <v>3813</v>
+        <v>3811</v>
       </c>
       <c r="B8" s="113"/>
       <c r="C8" s="113"/>
-      <c r="D8" s="113"/>
-      <c r="E8" s="128"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D8" s="128"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="119" t="s">
         <v>3806</v>
       </c>
       <c r="B9" s="119">
         <v>84220022</v>
       </c>
-      <c r="C9" s="129" t="s">
-        <v>3807</v>
-      </c>
-      <c r="D9" s="130">
-        <v>44435</v>
-      </c>
-      <c r="E9" s="131"/>
-    </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="129"/>
+      <c r="D9" s="130"/>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="118"/>
       <c r="B10" s="113"/>
       <c r="C10" s="113"/>
       <c r="D10" s="113"/>
-      <c r="E10" s="113"/>
-    </row>
-    <row r="11" spans="1:8" s="114" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:7" s="114" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="119" t="s">
         <v>3804</v>
       </c>
@@ -13459,140 +13428,121 @@
       <c r="C11" s="116" t="s">
         <v>3805</v>
       </c>
-      <c r="D11" s="145"/>
-      <c r="E11" s="145"/>
-      <c r="F11" s="132"/>
-      <c r="H11" s="115"/>
-    </row>
-    <row r="12" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="140"/>
+      <c r="E11" s="131"/>
+      <c r="G11" s="115"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="119"/>
       <c r="B12" s="119"/>
       <c r="C12" s="119"/>
       <c r="D12" s="119"/>
-      <c r="E12" s="119"/>
-    </row>
-    <row r="13" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="117"/>
       <c r="B13" s="117"/>
       <c r="C13" s="117"/>
       <c r="D13" s="117"/>
-      <c r="E13" s="117"/>
-    </row>
-    <row r="14" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="119"/>
       <c r="B14" s="119"/>
       <c r="C14" s="119"/>
       <c r="D14" s="119"/>
-      <c r="E14" s="119"/>
-    </row>
-    <row r="15" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="117"/>
       <c r="B15" s="117"/>
       <c r="C15" s="119"/>
       <c r="D15" s="119"/>
-      <c r="E15" s="119"/>
-    </row>
-    <row r="16" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="117"/>
       <c r="B16" s="117"/>
       <c r="C16" s="119"/>
       <c r="D16" s="119"/>
-      <c r="E16" s="119"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="118"/>
       <c r="B17" s="113"/>
-      <c r="C17" s="143"/>
-      <c r="D17" s="143"/>
-      <c r="E17" s="143"/>
-    </row>
-    <row r="18" spans="1:12" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="133" t="s">
+      <c r="C17" s="149"/>
+      <c r="D17" s="149"/>
+    </row>
+    <row r="18" spans="1:11" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="132" t="s">
+        <v>3812</v>
+      </c>
+      <c r="B18" s="133" t="s">
         <v>3814</v>
       </c>
-      <c r="B18" s="134" t="s">
-        <v>3816</v>
-      </c>
-      <c r="C18" s="135" t="s">
-        <v>3815</v>
-      </c>
-      <c r="D18" s="136"/>
-      <c r="E18" s="135" t="s">
+      <c r="C18" s="134" t="s">
+        <v>3813</v>
+      </c>
+      <c r="D18" s="134" t="s">
         <v>3796</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="152"/>
-      <c r="B19" s="153">
+    <row r="19" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="144"/>
+      <c r="B19" s="145">
         <v>9781877419164</v>
       </c>
-      <c r="C19" s="154"/>
-      <c r="D19" s="155"/>
-      <c r="E19" s="156">
+      <c r="C19" s="146"/>
+      <c r="D19" s="147">
         <v>1</v>
       </c>
-      <c r="L19" s="111"/>
-    </row>
-    <row r="20" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="137"/>
-      <c r="B20" s="138"/>
-      <c r="C20" s="139"/>
-      <c r="D20" s="140"/>
-      <c r="E20" s="141"/>
-      <c r="L20" s="111"/>
-    </row>
-    <row r="21" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="149" t="s">
-        <v>3811</v>
-      </c>
-      <c r="B21" s="149"/>
-      <c r="E21" s="121"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="147" t="s">
+      <c r="K19" s="111"/>
+    </row>
+    <row r="20" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="135"/>
+      <c r="B20" s="136"/>
+      <c r="C20" s="137"/>
+      <c r="D20" s="138"/>
+      <c r="K20" s="111"/>
+    </row>
+    <row r="21" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="153" t="s">
+        <v>3809</v>
+      </c>
+      <c r="B21" s="153"/>
+      <c r="D21" s="121"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="151" t="s">
+        <v>3807</v>
+      </c>
+      <c r="B22" s="152"/>
+      <c r="C22" s="116" t="s">
         <v>3808</v>
       </c>
-      <c r="B22" s="148"/>
-      <c r="C22" s="116" t="s">
-        <v>3809</v>
-      </c>
-      <c r="D22" s="148" t="s">
+      <c r="D22" s="142"/>
+    </row>
+    <row r="23" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A23" s="150" t="s">
         <v>3810</v>
       </c>
-      <c r="E22" s="148"/>
-    </row>
-    <row r="23" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A23" s="144" t="s">
-        <v>3812</v>
-      </c>
-      <c r="B23" s="144" t="s">
+      <c r="B23" s="150" t="s">
         <v>3795</v>
       </c>
-      <c r="C23" s="144"/>
-      <c r="D23" s="144"/>
-      <c r="E23" s="144" t="s">
+      <c r="C23" s="150"/>
+      <c r="D23" s="150" t="s">
         <v>3795</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="142"/>
-      <c r="B24" s="142"/>
-      <c r="C24" s="142"/>
-      <c r="D24" s="142"/>
-      <c r="E24" s="142"/>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="148"/>
+      <c r="B24" s="148"/>
+      <c r="C24" s="148"/>
+      <c r="D24" s="148"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D7:E7"/>
+  <mergeCells count="6">
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A23:D23"/>
     <mergeCell ref="A22:B22"/>
-    <mergeCell ref="D22:E22"/>
     <mergeCell ref="A21:B21"/>
-    <mergeCell ref="D6:E6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A22" r:id="rId1" xr:uid="{6C9DB83A-6524-4367-83E6-B3957F6154B3}"/>

</xml_diff>